<commit_message>
Fixed matching between woman and child
</commit_message>
<xml_diff>
--- a/app/config/tables/GRAVIDA/forms/GRAVIDA/GRAVIDA.xlsx
+++ b/app/config/tables/GRAVIDA/forms/GRAVIDA/GRAVIDA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1930E36-C9A5-4299-B18A-FB585B5C6EFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B796CE83-B8FE-41C4-AC60-E2204D746159}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="700" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="449">
   <si>
     <t>setting_name</t>
   </si>
@@ -1231,24 +1231,6 @@
     <t>&lt;b&gt;Registro de gravidez: {{data.nome}} - Nas: {{calculates.displayMifdnasc}}&lt;b&gt;</t>
   </si>
   <si>
-    <t>&lt;b&gt;2nd pregnancy visit: {{data.nome}} - Dob: {{calculates.displayMifdnasc}}&lt;b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;2ª visita de gravidez: {{data.nome}} - Nas: {{calculates.displayMifdnasc}}&lt;b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Pregnancy visit: {{data.nome}} - Dob: {{calculates.displayMifdnasc}}&lt;b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Visita de gravidez: {{data.nome}} - Nas: {{calculates.displayMifdnasc}}&lt;b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;After childbirth: {{data.nome}} - Dob: {{calculates.displayMifdnasc}}&lt;b&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Depois de parto: {{data.nome}} - Nas: {{calculates.displayMifdnasc}}&lt;b&gt;</t>
-  </si>
-  <si>
     <t>Maternal middle upper arm circumference</t>
   </si>
   <si>
@@ -1388,6 +1370,30 @@
   </si>
   <si>
     <t>display.hide_delete_button</t>
+  </si>
+  <si>
+    <t>adate.display(data('REGDIA'))</t>
+  </si>
+  <si>
+    <t>displayREGDIA</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Pregnancy visit: {{data.nome}} - Dob: {{calculates.displayREGDIA}}&lt;b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Visita de gravidez: {{data.nome}} - Nas: {{calculates.displayREGDIA}}&lt;b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;2nd pregnancy visit: {{data.nome}} - Dob: {{calculates.displayREGDIA}}&lt;b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;2ª visita de gravidez: {{data.nome}} - Nas: {{calculates.displayREGDIA}}&lt;b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;After childbirth: {{data.nome}} - Dob: {{calculates.displayREGDIA}}&lt;b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Depois de parto: {{data.nome}} - Nas: {{calculates.displayREGDIA}}&lt;b&gt;</t>
   </si>
 </sst>
 </file>
@@ -2720,9 +2726,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:N83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3766,9 +3772,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42B4652-1939-4CCD-AEEB-1868D449AB6E}">
   <dimension ref="A1:O89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3830,10 +3836,10 @@
         <v>300</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -3956,19 +3962,19 @@
         <v>365</v>
       </c>
       <c r="G11" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="H11" t="s">
         <v>245</v>
       </c>
       <c r="K11" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="L11" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="M11" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -4044,10 +4050,10 @@
         <v>327</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="H21" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -4146,7 +4152,7 @@
         <v>28</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H33" t="s">
         <v>40</v>
@@ -4166,13 +4172,13 @@
         <v>42</v>
       </c>
       <c r="K34" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="L34" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="M34" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
@@ -4197,13 +4203,13 @@
         <v>41</v>
       </c>
       <c r="K36" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="L36" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="M36" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
@@ -4345,7 +4351,7 @@
         <v>28</v>
       </c>
       <c r="G53" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H53" t="s">
         <v>43</v>
@@ -4453,7 +4459,7 @@
         <v>28</v>
       </c>
       <c r="G65" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="H65" t="s">
         <v>44</v>
@@ -4572,13 +4578,13 @@
         <v>329</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="H78" t="s">
         <v>46</v>
       </c>
       <c r="N78" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.25">
@@ -4612,10 +4618,10 @@
         <v>28</v>
       </c>
       <c r="G83" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="H83" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
@@ -4658,10 +4664,10 @@
         <v>383</v>
       </c>
       <c r="G88" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="H88" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
@@ -4681,7 +4687,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K46" sqref="K46"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4743,7 +4749,7 @@
         <v>300</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -4764,10 +4770,10 @@
         <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>396</v>
+        <v>443</v>
       </c>
       <c r="H3" t="s">
-        <v>397</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -4880,10 +4886,10 @@
         <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>394</v>
+        <v>445</v>
       </c>
       <c r="H11" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -4981,10 +4987,10 @@
         <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>394</v>
+        <v>445</v>
       </c>
       <c r="H20" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -4995,19 +5001,19 @@
         <v>362</v>
       </c>
       <c r="G21" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="H21" t="s">
         <v>245</v>
       </c>
       <c r="K21" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="L21" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="M21" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -5066,10 +5072,10 @@
         <v>28</v>
       </c>
       <c r="G30" t="s">
-        <v>394</v>
+        <v>445</v>
       </c>
       <c r="H30" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -5083,10 +5089,10 @@
         <v>342</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="H31" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -5104,10 +5110,10 @@
         <v>28</v>
       </c>
       <c r="G34" t="s">
-        <v>394</v>
+        <v>445</v>
       </c>
       <c r="H34" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
@@ -5174,10 +5180,10 @@
         <v>28</v>
       </c>
       <c r="G42" t="s">
-        <v>394</v>
+        <v>445</v>
       </c>
       <c r="H42" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
@@ -5185,7 +5191,7 @@
         <v>28</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="H43" t="s">
         <v>40</v>
@@ -5205,13 +5211,13 @@
         <v>42</v>
       </c>
       <c r="K44" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="L44" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="M44" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
@@ -5236,13 +5242,13 @@
         <v>41</v>
       </c>
       <c r="K46" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="L46" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="M46" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
@@ -5265,10 +5271,10 @@
         <v>28</v>
       </c>
       <c r="G50" t="s">
-        <v>394</v>
+        <v>445</v>
       </c>
       <c r="H50" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
@@ -5373,10 +5379,10 @@
         <v>28</v>
       </c>
       <c r="G62" t="s">
-        <v>394</v>
+        <v>445</v>
       </c>
       <c r="H62" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
@@ -5384,7 +5390,7 @@
         <v>28</v>
       </c>
       <c r="G63" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H63" t="s">
         <v>43</v>
@@ -5481,10 +5487,10 @@
         <v>28</v>
       </c>
       <c r="G74" t="s">
-        <v>394</v>
+        <v>445</v>
       </c>
       <c r="H74" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
@@ -5492,7 +5498,7 @@
         <v>28</v>
       </c>
       <c r="G75" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="H75" t="s">
         <v>44</v>
@@ -5597,10 +5603,10 @@
         <v>28</v>
       </c>
       <c r="G87" t="s">
-        <v>394</v>
+        <v>445</v>
       </c>
       <c r="H87" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -5611,13 +5617,13 @@
         <v>360</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="H88" t="s">
         <v>46</v>
       </c>
       <c r="N88" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -5640,10 +5646,10 @@
         <v>28</v>
       </c>
       <c r="G92" t="s">
-        <v>394</v>
+        <v>445</v>
       </c>
       <c r="H92" t="s">
-        <v>395</v>
+        <v>446</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -5654,10 +5660,10 @@
         <v>384</v>
       </c>
       <c r="G93" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="H93" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -5680,9 +5686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D665D096-BD70-4F59-A80B-B0F9CAA299C4}">
   <dimension ref="A1:N162"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5744,7 +5750,7 @@
         <v>300</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -5762,10 +5768,10 @@
         <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H3" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -5824,10 +5830,10 @@
         <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H8" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -5932,10 +5938,10 @@
         <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H20" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -5949,7 +5955,7 @@
         <v>116</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="H21" t="s">
         <v>246</v>
@@ -5970,10 +5976,10 @@
         <v>28</v>
       </c>
       <c r="G24" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H24" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -5984,19 +5990,19 @@
         <v>117</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="H25" t="s">
         <v>247</v>
       </c>
       <c r="K25" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="L25" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="M25" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -6023,10 +6029,10 @@
         <v>28</v>
       </c>
       <c r="G29" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H29" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -6108,10 +6114,10 @@
         <v>28</v>
       </c>
       <c r="G39" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H39" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -6143,10 +6149,10 @@
         <v>28</v>
       </c>
       <c r="G43" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H43" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -6181,10 +6187,10 @@
         <v>28</v>
       </c>
       <c r="G47" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H47" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -6219,10 +6225,10 @@
         <v>28</v>
       </c>
       <c r="G51" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H51" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
@@ -6236,10 +6242,10 @@
         <v>141</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="H52" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
@@ -6258,10 +6264,10 @@
         <v>143</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="H54" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
@@ -6284,10 +6290,10 @@
         <v>28</v>
       </c>
       <c r="G58" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H58" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
@@ -6295,7 +6301,7 @@
         <v>28</v>
       </c>
       <c r="G59" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="H59" t="s">
         <v>45</v>
@@ -6392,10 +6398,10 @@
         <v>28</v>
       </c>
       <c r="G70" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H70" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
@@ -6403,7 +6409,7 @@
         <v>28</v>
       </c>
       <c r="G71" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H71" t="s">
         <v>43</v>
@@ -6500,10 +6506,10 @@
         <v>28</v>
       </c>
       <c r="G82" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H82" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
@@ -6511,7 +6517,7 @@
         <v>28</v>
       </c>
       <c r="G83" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="H83" t="s">
         <v>44</v>
@@ -6608,10 +6614,10 @@
         <v>28</v>
       </c>
       <c r="G94" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H94" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
@@ -6628,7 +6634,7 @@
         <v>152</v>
       </c>
       <c r="H95" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
@@ -6646,10 +6652,10 @@
         <v>28</v>
       </c>
       <c r="G98" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H98" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -6697,10 +6703,10 @@
         <v>28</v>
       </c>
       <c r="G103" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H103" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -6824,10 +6830,10 @@
         <v>28</v>
       </c>
       <c r="G114" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H114" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
@@ -6872,10 +6878,10 @@
         <v>28</v>
       </c>
       <c r="G119" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H119" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
@@ -6890,7 +6896,7 @@
         <v>282</v>
       </c>
       <c r="G120" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="H120" t="s">
         <v>283</v>
@@ -6914,7 +6920,7 @@
         <v>285</v>
       </c>
       <c r="G122" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="H122" t="s">
         <v>286</v>
@@ -6948,10 +6954,10 @@
         <v>28</v>
       </c>
       <c r="G127" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H127" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
@@ -6994,10 +7000,10 @@
         <v>28</v>
       </c>
       <c r="G132" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H132" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="133" spans="2:14" x14ac:dyDescent="0.25">
@@ -7049,10 +7055,10 @@
         <v>28</v>
       </c>
       <c r="G138" s="9" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H138" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="139" spans="2:14" x14ac:dyDescent="0.25">
@@ -7104,10 +7110,10 @@
         <v>28</v>
       </c>
       <c r="G144" s="9" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H144" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.25">
@@ -7159,10 +7165,10 @@
         <v>28</v>
       </c>
       <c r="G150" s="9" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H150" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.25">
@@ -7228,10 +7234,10 @@
         <v>28</v>
       </c>
       <c r="G160" t="s">
-        <v>398</v>
+        <v>447</v>
       </c>
       <c r="H160" t="s">
-        <v>399</v>
+        <v>448</v>
       </c>
     </row>
     <row r="161" spans="2:8" x14ac:dyDescent="0.25">
@@ -7242,10 +7248,10 @@
         <v>385</v>
       </c>
       <c r="G161" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="H161" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="162" spans="2:8" x14ac:dyDescent="0.25">
@@ -7260,11 +7266,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3979F510-C769-4227-AA22-F1F6C93E2BBE}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7287,6 +7293,14 @@
       </c>
       <c r="B2" s="17" t="s">
         <v>389</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B3" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -7528,24 +7542,24 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="B2" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C2" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>